<commit_message>
good progress on app 31/07
</commit_message>
<xml_diff>
--- a/django_proj/data/letters spreadsheet.xlsx
+++ b/django_proj/data/letters spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\OneDrive\Documents\wsl\git\Letter_tracking\django_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{310F22D4-49DE-4996-A57E-1C3F93D54CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF9963-A520-48DE-93F4-D1E5B2FD77C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1888E834-CA7B-44E3-B669-379879081EE9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1888E834-CA7B-44E3-B669-379879081EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Estadísticas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Seguimiento!$A$8:$T$869</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Seguimiento!$A$8:$T$1082</definedName>
     <definedName name="Accion">Catálogos!$N$3:$N$6</definedName>
     <definedName name="CamaraParticipa">Catálogos!$G$3:$G$4</definedName>
     <definedName name="Especificos">Catálogos!$C$3:$C$22</definedName>
@@ -29,7 +29,6 @@
     <definedName name="Temas">Catálogos!$B$3:$B$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1652,7 +1651,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1762,6 +1761,14 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1829,10 +1836,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1937,6 +1945,9 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1956,7 +1967,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2276,9 +2288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18F1EDA-44DE-49BC-85DA-C19136B14E22}">
   <dimension ref="A2:T1082"/>
   <sheetViews>
-    <sheetView zoomScale="41" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -2305,25 +2317,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>506</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="I3" s="41" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="I3" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="40">
+      <c r="J3" s="42"/>
+      <c r="K3" s="41">
         <f>SUBTOTAL(2,$A:$A)</f>
         <v>92</v>
       </c>
@@ -2332,24 +2344,24 @@
       <c r="N3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="40"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="26"/>
       <c r="M4" s="24"/>
       <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="J5" s="28"/>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
@@ -49614,7 +49626,7 @@
       </c>
       <c r="B832" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>1930.05.15.B.D.COVID-19</v>
+        <v>2020.05.15.B.D.COVID-19</v>
       </c>
       <c r="C832" s="31" t="s">
         <v>24</v>
@@ -49623,7 +49635,7 @@
         <v>8</v>
       </c>
       <c r="E832" s="37">
-        <v>11093</v>
+        <v>43966</v>
       </c>
       <c r="F832" s="31" t="s">
         <v>1</v>
@@ -49675,7 +49687,7 @@
       <c r="A833" s="31"/>
       <c r="B833" s="31" t="str">
         <f t="shared" si="24"/>
-        <v>1930.05.15.B.D.COVID-19</v>
+        <v>2020.05.15.B.D.COVID-19</v>
       </c>
       <c r="C833" s="31" t="s">
         <v>24</v>
@@ -49684,7 +49696,7 @@
         <v>8</v>
       </c>
       <c r="E833" s="37">
-        <v>11093</v>
+        <v>43966</v>
       </c>
       <c r="F833" s="31" t="s">
         <v>1</v>
@@ -52262,7 +52274,7 @@
         <f>INDEX(Catálogos!$L$3:$L$537,MATCH(Seguimiento!N876,NombreLegislador,0))</f>
         <v>D</v>
       </c>
-      <c r="Q876" s="33" t="s">
+      <c r="Q876" s="40" t="s">
         <v>469</v>
       </c>
       <c r="R876" s="33" t="s">
@@ -57226,7 +57238,7 @@
     <row r="961" spans="1:20" s="38" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A961" s="31"/>
       <c r="B961" s="31" t="str">
-        <f t="shared" si="26"/>
+        <f>CONCATENATE(YEAR(E961),".",TEXT(E961,"mm"),".",TEXT(E961,"dd"),".",(IF(K961="Bicameral","B",IF(K961="Cámara","C","S"))),".",IF(L961="Bipartidista","B",IF(L961="Demócrata","D","R")),".",C961)</f>
         <v>2020.07.09.B.D.Migración</v>
       </c>
       <c r="C961" s="31" t="s">
@@ -61794,7 +61806,7 @@
       <c r="T1082" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A8:T869" xr:uid="{B364259B-C9C9-42CB-AC4F-8396199F50F8}"/>
+  <autoFilter ref="A8:T1082" xr:uid="{B364259B-C9C9-42CB-AC4F-8396199F50F8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:R54">
     <sortCondition ref="E8"/>
   </sortState>
@@ -62961,9 +62973,10 @@
     <hyperlink ref="Q138" r:id="rId14" xr:uid="{C5B6656C-E1E4-4186-A578-78066B12D3A2}"/>
     <hyperlink ref="Q139" r:id="rId15" xr:uid="{E8591C1C-6C93-4F70-8525-A7AF60B327A3}"/>
     <hyperlink ref="Q488" r:id="rId16" xr:uid="{A28C1CCC-1C75-49BF-8BF6-DAD16CCBD134}"/>
+    <hyperlink ref="Q876" r:id="rId17" xr:uid="{20AC614E-1FB6-4183-AC9F-9B6CEDC024EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -65391,7 +65404,7 @@
   <dimension ref="A2:N104"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="F8" sqref="F5:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -67013,7 +67026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B2A44-9C9D-447E-8326-123C92B0CB51}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -67037,11 +67050,11 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="44" t="s">
         <v>532</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="G3" s="11"/>
@@ -67059,10 +67072,10 @@
       <c r="E4" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="45" t="s">
         <v>526</v>
       </c>
-      <c r="H4" s="44"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="39"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.4">
@@ -67094,10 +67107,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="16"/>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="46" t="s">
         <v>527</v>
       </c>
-      <c r="H6" s="45"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="17">
         <f>SUM(H9:$I$11)</f>
         <v>0</v>

</xml_diff>